<commit_message>
Add note regarding AC/DC coupling
</commit_message>
<xml_diff>
--- a/matrixmixer-active-4x4.xlsx
+++ b/matrixmixer-active-4x4.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
   <si>
     <t xml:space="preserve">Qty</t>
   </si>
@@ -179,6 +179,15 @@
   </si>
   <si>
     <t xml:space="preserve">TL074/084 recommended – any pin-compatible quad op-amp should work.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOTE: populate JP1-4 depending on whether you want the inputs to be AC or DC coupled. For DC coupling, wire links or zero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ohm links will work. For AC coupling, use a 100nF ceramic capacitor – if you plan to exploit mixer feedback then AC coupling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is recommended in order to prevent the op-amps latching up.</t>
   </si>
 </sst>
 </file>
@@ -290,10 +299,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -303,7 +312,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="106.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="41.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="41.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="101.06"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
@@ -558,6 +567,21 @@
       </c>
       <c r="G12" s="0" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E15" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E16" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E17" s="0" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>